<commit_message>
added scope 1, stationary factors
</commit_message>
<xml_diff>
--- a/Raw_eGRID_EF_1.xlsx
+++ b/Raw_eGRID_EF_1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RituGothwal\Stok LLC\Python Scripts\Emission factor tool\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ebs1-my.sharepoint.com/personal/ritu_stok_com/Documents/Ritu/Python Scripts/Carbon_team_Scripts/Emission_factor_tool/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB31CA3F-A5DC-4EA1-BF05-0E89501011C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{FB31CA3F-A5DC-4EA1-BF05-0E89501011C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{469832B8-415E-4DF7-8CA7-F785CA7DE460}"/>
   <bookViews>
-    <workbookView xWindow="6192" yWindow="2436" windowWidth="23040" windowHeight="12120" xr2:uid="{684B57A3-FFB1-4E11-B6A1-72CE2EF8511A}"/>
+    <workbookView xWindow="-30828" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{684B57A3-FFB1-4E11-B6A1-72CE2EF8511A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1051,7 +1051,7 @@
   <dimension ref="A1:J57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F50" sqref="F50"/>
+      <selection activeCell="G1" sqref="G1:J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1061,7 +1061,7 @@
     <col min="3" max="3" width="15.44140625" customWidth="1"/>
     <col min="4" max="4" width="12.6640625" customWidth="1"/>
     <col min="5" max="5" width="13.33203125" customWidth="1"/>
-    <col min="6" max="6" width="16.109375" customWidth="1"/>
+    <col min="6" max="6" width="24.33203125" customWidth="1"/>
     <col min="7" max="7" width="14.77734375" customWidth="1"/>
     <col min="8" max="8" width="25.109375" customWidth="1"/>
     <col min="9" max="9" width="19.88671875" customWidth="1"/>

</xml_diff>

<commit_message>
improved app with app_9 file
</commit_message>
<xml_diff>
--- a/Raw_eGRID_EF_1.xlsx
+++ b/Raw_eGRID_EF_1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ebs1-my.sharepoint.com/personal/ritu_stok_com/Documents/Ritu/Python Scripts/Carbon_team_Scripts/Emission_factor_tool/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{FB31CA3F-A5DC-4EA1-BF05-0E89501011C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{469832B8-415E-4DF7-8CA7-F785CA7DE460}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="13_ncr:1_{FB31CA3F-A5DC-4EA1-BF05-0E89501011C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D136C446-02EE-45F2-A839-2371D8EC5A1C}"/>
   <bookViews>
-    <workbookView xWindow="-30828" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{684B57A3-FFB1-4E11-B6A1-72CE2EF8511A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{684B57A3-FFB1-4E11-B6A1-72CE2EF8511A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -312,6 +312,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="165" formatCode="#,##0.0"/>
+    <numFmt numFmtId="167" formatCode="0.000"/>
+  </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -674,7 +678,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -689,8 +693,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -702,18 +704,19 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="4" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="4" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="4" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1050,8 +1053,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1438D341-D9D5-4BED-8D37-889B5147565D}">
   <dimension ref="A1:J57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:J4"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30:E57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1081,22 +1084,22 @@
       <c r="D1" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="E1" s="25" t="s">
+      <c r="E1" s="17" t="s">
         <v>59</v>
       </c>
       <c r="F1" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="I1" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="J1" s="9" t="s">
         <v>62</v>
       </c>
     </row>
@@ -1107,28 +1110,28 @@
       <c r="B2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="8">
+      <c r="C2" s="18">
         <v>1067.7</v>
       </c>
-      <c r="D2" s="9">
+      <c r="D2" s="22">
         <v>9.0999999999999998E-2</v>
       </c>
-      <c r="E2" s="26">
+      <c r="E2" s="23">
         <v>1.2E-2</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="G2" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="H2" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="I2" s="10">
-        <v>2021</v>
-      </c>
-      <c r="J2" s="10">
+      <c r="G2" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="I2" s="8">
+        <v>2021</v>
+      </c>
+      <c r="J2" s="8">
         <v>2022</v>
       </c>
     </row>
@@ -1139,28 +1142,28 @@
       <c r="B3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="9">
+      <c r="C3" s="18">
         <v>485.2</v>
       </c>
-      <c r="D3" s="9">
+      <c r="D3" s="22">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="E3" s="26">
+      <c r="E3" s="23">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="F3" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="G3" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="H3" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="I3" s="10">
-        <v>2021</v>
-      </c>
-      <c r="J3" s="10">
+      <c r="G3" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="I3" s="8">
+        <v>2021</v>
+      </c>
+      <c r="J3" s="8">
         <v>2022</v>
       </c>
     </row>
@@ -1171,28 +1174,28 @@
       <c r="B4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="9">
+      <c r="C4" s="18">
         <v>819.7</v>
       </c>
-      <c r="D4" s="9">
+      <c r="D4" s="22">
         <v>5.1999999999999998E-2</v>
       </c>
-      <c r="E4" s="26">
+      <c r="E4" s="23">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="F4" s="12" t="s">
+      <c r="F4" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="G4" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="H4" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="I4" s="10">
-        <v>2021</v>
-      </c>
-      <c r="J4" s="10">
+      <c r="G4" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="I4" s="8">
+        <v>2021</v>
+      </c>
+      <c r="J4" s="8">
         <v>2022</v>
       </c>
     </row>
@@ -1203,28 +1206,28 @@
       <c r="B5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="9">
+      <c r="C5" s="18">
         <v>531.70000000000005</v>
       </c>
-      <c r="D5" s="9">
+      <c r="D5" s="22">
         <v>3.1E-2</v>
       </c>
-      <c r="E5" s="26">
+      <c r="E5" s="23">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="F5" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="G5" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="H5" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="I5" s="10">
-        <v>2021</v>
-      </c>
-      <c r="J5" s="10">
+      <c r="G5" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="I5" s="8">
+        <v>2021</v>
+      </c>
+      <c r="J5" s="8">
         <v>2022</v>
       </c>
     </row>
@@ -1235,28 +1238,28 @@
       <c r="B6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="9">
+      <c r="C6" s="18">
         <v>813.6</v>
       </c>
-      <c r="D6" s="9">
+      <c r="D6" s="22">
         <v>5.3999999999999999E-2</v>
       </c>
-      <c r="E6" s="26">
+      <c r="E6" s="23">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="F6" s="12" t="s">
+      <c r="F6" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="G6" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="H6" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="I6" s="10">
-        <v>2021</v>
-      </c>
-      <c r="J6" s="10">
+      <c r="G6" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="I6" s="8">
+        <v>2021</v>
+      </c>
+      <c r="J6" s="8">
         <v>2022</v>
       </c>
     </row>
@@ -1267,28 +1270,28 @@
       <c r="B7" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="9">
+      <c r="C7" s="18">
         <v>832.9</v>
       </c>
-      <c r="D7" s="9">
+      <c r="D7" s="22">
         <v>5.2999999999999999E-2</v>
       </c>
-      <c r="E7" s="26">
+      <c r="E7" s="23">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="F7" s="12" t="s">
+      <c r="F7" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="G7" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="H7" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="I7" s="10">
-        <v>2021</v>
-      </c>
-      <c r="J7" s="10">
+      <c r="G7" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="I7" s="8">
+        <v>2021</v>
+      </c>
+      <c r="J7" s="8">
         <v>2022</v>
       </c>
     </row>
@@ -1299,28 +1302,28 @@
       <c r="B8" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="8">
+      <c r="C8" s="18">
         <v>1134.4000000000001</v>
       </c>
-      <c r="D8" s="9">
+      <c r="D8" s="22">
         <v>0.13500000000000001</v>
       </c>
-      <c r="E8" s="26">
+      <c r="E8" s="23">
         <v>2.1000000000000001E-2</v>
       </c>
-      <c r="F8" s="12" t="s">
+      <c r="F8" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="G8" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="H8" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="I8" s="10">
-        <v>2021</v>
-      </c>
-      <c r="J8" s="10">
+      <c r="G8" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="I8" s="8">
+        <v>2021</v>
+      </c>
+      <c r="J8" s="8">
         <v>2022</v>
       </c>
     </row>
@@ -1331,28 +1334,28 @@
       <c r="B9" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="8">
+      <c r="C9" s="18">
         <v>1633.1</v>
       </c>
-      <c r="D9" s="9">
+      <c r="D9" s="22">
         <v>0.17599999999999999</v>
       </c>
-      <c r="E9" s="26">
+      <c r="E9" s="23">
         <v>2.7E-2</v>
       </c>
-      <c r="F9" s="12" t="s">
+      <c r="F9" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="G9" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="H9" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="I9" s="10">
-        <v>2021</v>
-      </c>
-      <c r="J9" s="10">
+      <c r="G9" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="I9" s="8">
+        <v>2021</v>
+      </c>
+      <c r="J9" s="8">
         <v>2022</v>
       </c>
     </row>
@@ -1363,28 +1366,28 @@
       <c r="B10" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="8">
+      <c r="C10" s="18">
         <v>1582.1</v>
       </c>
-      <c r="D10" s="9">
+      <c r="D10" s="22">
         <v>0.14799999999999999</v>
       </c>
-      <c r="E10" s="26">
+      <c r="E10" s="23">
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="F10" s="12" t="s">
+      <c r="F10" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="G10" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="H10" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="I10" s="10">
-        <v>2021</v>
-      </c>
-      <c r="J10" s="10">
+      <c r="G10" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="I10" s="8">
+        <v>2021</v>
+      </c>
+      <c r="J10" s="8">
         <v>2022</v>
       </c>
     </row>
@@ -1395,28 +1398,28 @@
       <c r="B11" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="9">
+      <c r="C11" s="18">
         <v>995.8</v>
       </c>
-      <c r="D11" s="9">
+      <c r="D11" s="22">
         <v>0.107</v>
       </c>
-      <c r="E11" s="26">
+      <c r="E11" s="23">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="F11" s="12" t="s">
+      <c r="F11" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="G11" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="H11" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="I11" s="10">
-        <v>2021</v>
-      </c>
-      <c r="J11" s="10">
+      <c r="G11" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="H11" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="I11" s="8">
+        <v>2021</v>
+      </c>
+      <c r="J11" s="8">
         <v>2022</v>
       </c>
     </row>
@@ -1427,28 +1430,28 @@
       <c r="B12" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="9">
+      <c r="C12" s="18">
         <v>539.4</v>
       </c>
-      <c r="D12" s="9">
+      <c r="D12" s="22">
         <v>7.1999999999999995E-2</v>
       </c>
-      <c r="E12" s="26">
+      <c r="E12" s="23">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="F12" s="12" t="s">
+      <c r="F12" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="G12" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="H12" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="I12" s="10">
-        <v>2021</v>
-      </c>
-      <c r="J12" s="10">
+      <c r="G12" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="H12" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="I12" s="8">
+        <v>2021</v>
+      </c>
+      <c r="J12" s="8">
         <v>2022</v>
       </c>
     </row>
@@ -1459,28 +1462,28 @@
       <c r="B13" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="9">
+      <c r="C13" s="18">
         <v>634.6</v>
       </c>
-      <c r="D13" s="9">
+      <c r="D13" s="22">
         <v>5.8000000000000003E-2</v>
       </c>
-      <c r="E13" s="26">
+      <c r="E13" s="23">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="F13" s="12" t="s">
+      <c r="F13" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="G13" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="H13" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="I13" s="10">
-        <v>2021</v>
-      </c>
-      <c r="J13" s="10">
+      <c r="G13" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="H13" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="I13" s="8">
+        <v>2021</v>
+      </c>
+      <c r="J13" s="8">
         <v>2022</v>
       </c>
     </row>
@@ -1491,28 +1494,28 @@
       <c r="B14" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="9">
+      <c r="C14" s="18">
         <v>816.8</v>
       </c>
-      <c r="D14" s="9">
+      <c r="D14" s="22">
         <v>1.9E-2</v>
       </c>
-      <c r="E14" s="26">
+      <c r="E14" s="23">
         <v>2E-3</v>
       </c>
-      <c r="F14" s="12" t="s">
+      <c r="F14" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="G14" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="H14" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="I14" s="10">
-        <v>2021</v>
-      </c>
-      <c r="J14" s="10">
+      <c r="G14" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="H14" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="I14" s="8">
+        <v>2021</v>
+      </c>
+      <c r="J14" s="8">
         <v>2022</v>
       </c>
     </row>
@@ -1523,28 +1526,28 @@
       <c r="B15" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C15" s="8">
+      <c r="C15" s="18">
         <v>1210.9000000000001</v>
       </c>
-      <c r="D15" s="9">
+      <c r="D15" s="22">
         <v>0.126</v>
       </c>
-      <c r="E15" s="26">
+      <c r="E15" s="23">
         <v>1.6E-2</v>
       </c>
-      <c r="F15" s="12" t="s">
+      <c r="F15" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="G15" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="H15" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="I15" s="10">
-        <v>2021</v>
-      </c>
-      <c r="J15" s="10">
+      <c r="G15" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="H15" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="I15" s="8">
+        <v>2021</v>
+      </c>
+      <c r="J15" s="8">
         <v>2022</v>
       </c>
     </row>
@@ -1555,28 +1558,28 @@
       <c r="B16" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="9">
+      <c r="C16" s="18">
         <v>233.1</v>
       </c>
-      <c r="D16" s="9">
+      <c r="D16" s="22">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="E16" s="26">
+      <c r="E16" s="23">
         <v>2E-3</v>
       </c>
-      <c r="F16" s="12" t="s">
+      <c r="F16" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="G16" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="H16" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="I16" s="10">
-        <v>2021</v>
-      </c>
-      <c r="J16" s="10">
+      <c r="G16" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="H16" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="I16" s="8">
+        <v>2021</v>
+      </c>
+      <c r="J16" s="8">
         <v>2022</v>
       </c>
     </row>
@@ -1587,28 +1590,28 @@
       <c r="B17" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="8">
+      <c r="C17" s="18">
         <v>1558</v>
       </c>
-      <c r="D17" s="9">
+      <c r="D17" s="22">
         <v>8.1000000000000003E-2</v>
       </c>
-      <c r="E17" s="26">
+      <c r="E17" s="23">
         <v>1.2999999999999999E-2</v>
       </c>
-      <c r="F17" s="12" t="s">
+      <c r="F17" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="G17" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="H17" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="I17" s="10">
-        <v>2021</v>
-      </c>
-      <c r="J17" s="10">
+      <c r="G17" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="H17" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="I17" s="8">
+        <v>2021</v>
+      </c>
+      <c r="J17" s="8">
         <v>2022</v>
       </c>
     </row>
@@ -1619,28 +1622,28 @@
       <c r="B18" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C18" s="9">
+      <c r="C18" s="18">
         <v>672.8</v>
       </c>
-      <c r="D18" s="9">
+      <c r="D18" s="22">
         <v>4.9000000000000002E-2</v>
       </c>
-      <c r="E18" s="26">
+      <c r="E18" s="23">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="F18" s="12" t="s">
+      <c r="F18" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="G18" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="H18" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="I18" s="10">
-        <v>2021</v>
-      </c>
-      <c r="J18" s="10">
+      <c r="G18" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="H18" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="I18" s="8">
+        <v>2021</v>
+      </c>
+      <c r="J18" s="8">
         <v>2022</v>
       </c>
     </row>
@@ -1651,28 +1654,28 @@
       <c r="B19" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C19" s="8">
+      <c r="C19" s="18">
         <v>1214.0999999999999</v>
       </c>
-      <c r="D19" s="9">
+      <c r="D19" s="22">
         <v>0.115</v>
       </c>
-      <c r="E19" s="26">
+      <c r="E19" s="23">
         <v>1.6E-2</v>
       </c>
-      <c r="F19" s="12" t="s">
+      <c r="F19" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="G19" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="H19" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="I19" s="10">
-        <v>2021</v>
-      </c>
-      <c r="J19" s="10">
+      <c r="G19" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="H19" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="I19" s="8">
+        <v>2021</v>
+      </c>
+      <c r="J19" s="8">
         <v>2022</v>
       </c>
     </row>
@@ -1683,28 +1686,28 @@
       <c r="B20" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C20" s="8">
+      <c r="C20" s="18">
         <v>1046.0999999999999</v>
       </c>
-      <c r="D20" s="9">
+      <c r="D20" s="22">
         <v>9.5000000000000001E-2</v>
       </c>
-      <c r="E20" s="26">
+      <c r="E20" s="23">
         <v>1.4E-2</v>
       </c>
-      <c r="F20" s="12" t="s">
+      <c r="F20" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="G20" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="H20" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="I20" s="10">
-        <v>2021</v>
-      </c>
-      <c r="J20" s="10">
+      <c r="G20" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="H20" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="I20" s="8">
+        <v>2021</v>
+      </c>
+      <c r="J20" s="8">
         <v>2022</v>
       </c>
     </row>
@@ -1715,28 +1718,28 @@
       <c r="B21" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="C21" s="8">
+      <c r="C21" s="18">
         <v>1158.9000000000001</v>
       </c>
-      <c r="D21" s="9">
+      <c r="D21" s="22">
         <v>0.109</v>
       </c>
-      <c r="E21" s="26">
+      <c r="E21" s="23">
         <v>1.6E-2</v>
       </c>
-      <c r="F21" s="12" t="s">
+      <c r="F21" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="G21" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="H21" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="I21" s="10">
-        <v>2021</v>
-      </c>
-      <c r="J21" s="10">
+      <c r="G21" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="H21" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="I21" s="8">
+        <v>2021</v>
+      </c>
+      <c r="J21" s="8">
         <v>2022</v>
       </c>
     </row>
@@ -1747,28 +1750,28 @@
       <c r="B22" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="C22" s="9">
+      <c r="C22" s="18">
         <v>991.7</v>
       </c>
-      <c r="D22" s="9">
+      <c r="D22" s="22">
         <v>0.108</v>
       </c>
-      <c r="E22" s="26">
+      <c r="E22" s="23">
         <v>1.6E-2</v>
       </c>
-      <c r="F22" s="12" t="s">
+      <c r="F22" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="G22" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="H22" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="I22" s="10">
-        <v>2021</v>
-      </c>
-      <c r="J22" s="10">
+      <c r="G22" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="H22" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="I22" s="8">
+        <v>2021</v>
+      </c>
+      <c r="J22" s="8">
         <v>2022</v>
       </c>
     </row>
@@ -1779,28 +1782,28 @@
       <c r="B23" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C23" s="8">
+      <c r="C23" s="18">
         <v>1031.5999999999999</v>
       </c>
-      <c r="D23" s="9">
+      <c r="D23" s="22">
         <v>0.08</v>
       </c>
-      <c r="E23" s="26">
+      <c r="E23" s="23">
         <v>1.2E-2</v>
       </c>
-      <c r="F23" s="12" t="s">
+      <c r="F23" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="G23" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="H23" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="I23" s="10">
-        <v>2021</v>
-      </c>
-      <c r="J23" s="10">
+      <c r="G23" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="H23" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="I23" s="8">
+        <v>2021</v>
+      </c>
+      <c r="J23" s="8">
         <v>2022</v>
       </c>
     </row>
@@ -1811,28 +1814,28 @@
       <c r="B24" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C24" s="9">
+      <c r="C24" s="18">
         <v>772.7</v>
       </c>
-      <c r="D24" s="9">
+      <c r="D24" s="22">
         <v>0.04</v>
       </c>
-      <c r="E24" s="26">
+      <c r="E24" s="23">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="F24" s="12" t="s">
+      <c r="F24" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="G24" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="H24" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="I24" s="10">
-        <v>2021</v>
-      </c>
-      <c r="J24" s="10">
+      <c r="G24" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="H24" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="I24" s="8">
+        <v>2021</v>
+      </c>
+      <c r="J24" s="8">
         <v>2022</v>
       </c>
     </row>
@@ -1843,28 +1846,28 @@
       <c r="B25" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C25" s="8">
+      <c r="C25" s="18">
         <v>1543</v>
       </c>
-      <c r="D25" s="9">
+      <c r="D25" s="22">
         <v>0.17100000000000001</v>
       </c>
-      <c r="E25" s="26">
+      <c r="E25" s="23">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="F25" s="12" t="s">
+      <c r="F25" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="G25" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="H25" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="I25" s="10">
-        <v>2021</v>
-      </c>
-      <c r="J25" s="10">
+      <c r="G25" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="H25" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="I25" s="8">
+        <v>2021</v>
+      </c>
+      <c r="J25" s="8">
         <v>2022</v>
       </c>
     </row>
@@ -1875,28 +1878,28 @@
       <c r="B26" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="C26" s="9">
+      <c r="C26" s="18">
         <v>891.9</v>
       </c>
-      <c r="D26" s="9">
+      <c r="D26" s="22">
         <v>6.7000000000000004E-2</v>
       </c>
-      <c r="E26" s="26">
+      <c r="E26" s="23">
         <v>0.01</v>
       </c>
-      <c r="F26" s="12" t="s">
+      <c r="F26" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="G26" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="H26" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="I26" s="10">
-        <v>2021</v>
-      </c>
-      <c r="J26" s="10">
+      <c r="G26" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="H26" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="I26" s="8">
+        <v>2021</v>
+      </c>
+      <c r="J26" s="8">
         <v>2022</v>
       </c>
     </row>
@@ -1907,28 +1910,28 @@
       <c r="B27" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="C27" s="9">
+      <c r="C27" s="18">
         <v>931.6</v>
       </c>
-      <c r="D27" s="9">
+      <c r="D27" s="22">
         <v>8.6999999999999994E-2</v>
       </c>
-      <c r="E27" s="26">
+      <c r="E27" s="23">
         <v>1.2999999999999999E-2</v>
       </c>
-      <c r="F27" s="12" t="s">
+      <c r="F27" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="G27" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="H27" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="I27" s="10">
-        <v>2021</v>
-      </c>
-      <c r="J27" s="10">
+      <c r="G27" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="H27" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="I27" s="8">
+        <v>2021</v>
+      </c>
+      <c r="J27" s="8">
         <v>2022</v>
       </c>
     </row>
@@ -1939,28 +1942,28 @@
       <c r="B28" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C28" s="9">
+      <c r="C28" s="18">
         <v>639.70000000000005</v>
       </c>
-      <c r="D28" s="9">
+      <c r="D28" s="22">
         <v>5.1999999999999998E-2</v>
       </c>
-      <c r="E28" s="26">
+      <c r="E28" s="23">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="F28" s="12" t="s">
+      <c r="F28" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="G28" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="H28" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="I28" s="10">
-        <v>2021</v>
-      </c>
-      <c r="J28" s="10">
+      <c r="G28" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="H28" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="I28" s="8">
+        <v>2021</v>
+      </c>
+      <c r="J28" s="8">
         <v>2022</v>
       </c>
     </row>
@@ -1971,924 +1974,924 @@
       <c r="B29" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="C29" s="9">
+      <c r="C29" s="18">
         <v>852.3</v>
       </c>
-      <c r="D29" s="9">
+      <c r="D29" s="22">
         <v>7.0999999999999994E-2</v>
       </c>
-      <c r="E29" s="26">
+      <c r="E29" s="23">
         <v>0.01</v>
       </c>
-      <c r="F29" s="12" t="s">
+      <c r="F29" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="G29" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="H29" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="I29" s="10">
-        <v>2021</v>
-      </c>
-      <c r="J29" s="10">
+      <c r="G29" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="H29" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="I29" s="8">
+        <v>2021</v>
+      </c>
+      <c r="J29" s="8">
         <v>2022</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A30" s="13" t="s">
+      <c r="A30" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="14" t="s">
+      <c r="B30" s="12" t="s">
         <v>3</v>
       </c>
       <c r="C30" s="19">
         <v>1229.5999999999999</v>
       </c>
-      <c r="D30" s="20">
+      <c r="D30" s="24">
         <v>0.12</v>
       </c>
-      <c r="E30" s="27">
+      <c r="E30" s="25">
         <v>1.6E-2</v>
       </c>
-      <c r="F30" s="12" t="s">
+      <c r="F30" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="G30" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="H30" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="I30" s="10">
-        <v>2021</v>
-      </c>
-      <c r="J30" s="10">
+      <c r="G30" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="H30" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="I30" s="8">
+        <v>2021</v>
+      </c>
+      <c r="J30" s="8">
         <v>2022</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A31" s="15" t="s">
+      <c r="A31" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B31" s="16" t="s">
+      <c r="B31" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C31" s="21">
+      <c r="C31" s="20">
         <v>1531.3</v>
       </c>
-      <c r="D31" s="9">
+      <c r="D31" s="22">
         <v>6.6000000000000003E-2</v>
       </c>
-      <c r="E31" s="26">
+      <c r="E31" s="23">
         <v>1.2E-2</v>
       </c>
-      <c r="F31" s="12" t="s">
+      <c r="F31" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="G31" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="H31" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="I31" s="10">
-        <v>2021</v>
-      </c>
-      <c r="J31" s="10">
+      <c r="G31" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="H31" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="I31" s="8">
+        <v>2021</v>
+      </c>
+      <c r="J31" s="8">
         <v>2022</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A32" s="15" t="s">
+      <c r="A32" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B32" s="16" t="s">
+      <c r="B32" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C32" s="21">
+      <c r="C32" s="20">
         <v>1227.5999999999999</v>
       </c>
-      <c r="D32" s="9">
+      <c r="D32" s="22">
         <v>6.7000000000000004E-2</v>
       </c>
-      <c r="E32" s="26">
+      <c r="E32" s="23">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="F32" s="12" t="s">
+      <c r="F32" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="G32" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="H32" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="I32" s="10">
-        <v>2021</v>
-      </c>
-      <c r="J32" s="10">
+      <c r="G32" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="H32" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="I32" s="8">
+        <v>2021</v>
+      </c>
+      <c r="J32" s="8">
         <v>2022</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A33" s="15" t="s">
+      <c r="A33" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B33" s="16" t="s">
+      <c r="B33" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C33" s="21">
+      <c r="C33" s="20">
         <v>1047.5</v>
       </c>
-      <c r="D33" s="9">
+      <c r="D33" s="22">
         <v>4.9000000000000002E-2</v>
       </c>
-      <c r="E33" s="26">
+      <c r="E33" s="23">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="F33" s="12" t="s">
+      <c r="F33" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="G33" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="H33" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="I33" s="10">
-        <v>2021</v>
-      </c>
-      <c r="J33" s="10">
+      <c r="G33" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="H33" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="I33" s="8">
+        <v>2021</v>
+      </c>
+      <c r="J33" s="8">
         <v>2022</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A34" s="15" t="s">
+      <c r="A34" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B34" s="16" t="s">
+      <c r="B34" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="C34" s="21">
+      <c r="C34" s="20">
         <v>1177.4000000000001</v>
       </c>
-      <c r="D34" s="9">
+      <c r="D34" s="22">
         <v>6.5000000000000002E-2</v>
       </c>
-      <c r="E34" s="26">
+      <c r="E34" s="23">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="F34" s="12" t="s">
+      <c r="F34" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="G34" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="H34" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="I34" s="10">
-        <v>2021</v>
-      </c>
-      <c r="J34" s="10">
+      <c r="G34" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="H34" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="I34" s="8">
+        <v>2021</v>
+      </c>
+      <c r="J34" s="8">
         <v>2022</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A35" s="15" t="s">
+      <c r="A35" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B35" s="16" t="s">
+      <c r="B35" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="C35" s="21">
+      <c r="C35" s="20">
         <v>1016.5</v>
       </c>
-      <c r="D35" s="9">
+      <c r="D35" s="22">
         <v>5.3999999999999999E-2</v>
       </c>
-      <c r="E35" s="26">
+      <c r="E35" s="23">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="F35" s="12" t="s">
+      <c r="F35" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="G35" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="H35" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="I35" s="10">
-        <v>2021</v>
-      </c>
-      <c r="J35" s="10">
+      <c r="G35" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="H35" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="I35" s="8">
+        <v>2021</v>
+      </c>
+      <c r="J35" s="8">
         <v>2022</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A36" s="15" t="s">
+      <c r="A36" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B36" s="16" t="s">
+      <c r="B36" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="C36" s="21">
+      <c r="C36" s="20">
         <v>1649.4</v>
       </c>
-      <c r="D36" s="9">
+      <c r="D36" s="22">
         <v>0.17599999999999999</v>
       </c>
-      <c r="E36" s="26">
+      <c r="E36" s="23">
         <v>2.7E-2</v>
       </c>
-      <c r="F36" s="12" t="s">
+      <c r="F36" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="G36" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="H36" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="I36" s="10">
-        <v>2021</v>
-      </c>
-      <c r="J36" s="10">
+      <c r="G36" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="H36" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="I36" s="8">
+        <v>2021</v>
+      </c>
+      <c r="J36" s="8">
         <v>2022</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A37" s="15" t="s">
+      <c r="A37" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="B37" s="16" t="s">
+      <c r="B37" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="C37" s="21">
+      <c r="C37" s="20">
         <v>1784</v>
       </c>
-      <c r="D37" s="9">
+      <c r="D37" s="22">
         <v>0.17199999999999999</v>
       </c>
-      <c r="E37" s="26">
+      <c r="E37" s="23">
         <v>2.7E-2</v>
       </c>
-      <c r="F37" s="12" t="s">
+      <c r="F37" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="G37" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="H37" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="I37" s="10">
-        <v>2021</v>
-      </c>
-      <c r="J37" s="10">
+      <c r="G37" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="H37" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="I37" s="8">
+        <v>2021</v>
+      </c>
+      <c r="J37" s="8">
         <v>2022</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A38" s="15" t="s">
+      <c r="A38" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B38" s="16" t="s">
+      <c r="B38" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C38" s="21">
+      <c r="C38" s="20">
         <v>1555.9</v>
       </c>
-      <c r="D38" s="9">
+      <c r="D38" s="22">
         <v>0.13300000000000001</v>
       </c>
-      <c r="E38" s="26">
+      <c r="E38" s="23">
         <v>1.9E-2</v>
       </c>
-      <c r="F38" s="12" t="s">
+      <c r="F38" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="G38" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="H38" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="I38" s="10">
-        <v>2021</v>
-      </c>
-      <c r="J38" s="10">
+      <c r="G38" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="H38" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="I38" s="8">
+        <v>2021</v>
+      </c>
+      <c r="J38" s="8">
         <v>2022</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A39" s="15" t="s">
+      <c r="A39" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B39" s="16" t="s">
+      <c r="B39" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="C39" s="21">
+      <c r="C39" s="20">
         <v>1808.3</v>
       </c>
-      <c r="D39" s="9">
+      <c r="D39" s="22">
         <v>0.183</v>
       </c>
-      <c r="E39" s="26">
+      <c r="E39" s="23">
         <v>2.5999999999999999E-2</v>
       </c>
-      <c r="F39" s="12" t="s">
+      <c r="F39" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="G39" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="H39" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="I39" s="10">
-        <v>2021</v>
-      </c>
-      <c r="J39" s="10">
+      <c r="G39" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="H39" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="I39" s="8">
+        <v>2021</v>
+      </c>
+      <c r="J39" s="8">
         <v>2022</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A40" s="15" t="s">
+      <c r="A40" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B40" s="16" t="s">
+      <c r="B40" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="C40" s="22">
+      <c r="C40" s="20">
         <v>900.5</v>
       </c>
-      <c r="D40" s="9">
+      <c r="D40" s="22">
         <v>7.2999999999999995E-2</v>
       </c>
-      <c r="E40" s="26">
+      <c r="E40" s="23">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="F40" s="12" t="s">
+      <c r="F40" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="G40" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="H40" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="I40" s="10">
-        <v>2021</v>
-      </c>
-      <c r="J40" s="10">
+      <c r="G40" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="H40" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="I40" s="8">
+        <v>2021</v>
+      </c>
+      <c r="J40" s="8">
         <v>2022</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A41" s="15" t="s">
+      <c r="A41" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B41" s="16" t="s">
+      <c r="B41" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="C41" s="21">
+      <c r="C41" s="20">
         <v>1545.7</v>
       </c>
-      <c r="D41" s="9">
+      <c r="D41" s="22">
         <v>0.13900000000000001</v>
       </c>
-      <c r="E41" s="26">
+      <c r="E41" s="23">
         <v>0.02</v>
       </c>
-      <c r="F41" s="12" t="s">
+      <c r="F41" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="G41" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="H41" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="I41" s="10">
-        <v>2021</v>
-      </c>
-      <c r="J41" s="10">
+      <c r="G41" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="H41" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="I41" s="8">
+        <v>2021</v>
+      </c>
+      <c r="J41" s="8">
         <v>2022</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A42" s="15" t="s">
+      <c r="A42" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="B42" s="16" t="s">
+      <c r="B42" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="C42" s="22">
+      <c r="C42" s="20">
         <v>930.8</v>
       </c>
-      <c r="D42" s="9">
+      <c r="D42" s="22">
         <v>0.02</v>
       </c>
-      <c r="E42" s="26">
+      <c r="E42" s="23">
         <v>2E-3</v>
       </c>
-      <c r="F42" s="12" t="s">
+      <c r="F42" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="G42" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="H42" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="I42" s="10">
-        <v>2021</v>
-      </c>
-      <c r="J42" s="10">
+      <c r="G42" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="H42" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="I42" s="8">
+        <v>2021</v>
+      </c>
+      <c r="J42" s="8">
         <v>2022</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A43" s="15" t="s">
+      <c r="A43" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B43" s="16" t="s">
+      <c r="B43" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="C43" s="21">
+      <c r="C43" s="20">
         <v>1317.3</v>
       </c>
-      <c r="D43" s="9">
+      <c r="D43" s="22">
         <v>0.04</v>
       </c>
-      <c r="E43" s="26">
+      <c r="E43" s="23">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="F43" s="12" t="s">
+      <c r="F43" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="G43" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="H43" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="I43" s="10">
-        <v>2021</v>
-      </c>
-      <c r="J43" s="10">
+      <c r="G43" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="H43" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="I43" s="8">
+        <v>2021</v>
+      </c>
+      <c r="J43" s="8">
         <v>2022</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A44" s="15" t="s">
+      <c r="A44" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="B44" s="16" t="s">
+      <c r="B44" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="C44" s="22">
+      <c r="C44" s="20">
         <v>880.7</v>
       </c>
-      <c r="D44" s="9">
+      <c r="D44" s="22">
         <v>4.7E-2</v>
       </c>
-      <c r="E44" s="26">
+      <c r="E44" s="23">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="F44" s="12" t="s">
+      <c r="F44" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="G44" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="H44" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="I44" s="10">
-        <v>2021</v>
-      </c>
-      <c r="J44" s="10">
+      <c r="G44" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="H44" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="I44" s="8">
+        <v>2021</v>
+      </c>
+      <c r="J44" s="8">
         <v>2022</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A45" s="15" t="s">
+      <c r="A45" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="B45" s="16" t="s">
+      <c r="B45" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="C45" s="21">
+      <c r="C45" s="20">
         <v>1618.1</v>
       </c>
-      <c r="D45" s="9">
+      <c r="D45" s="22">
         <v>0.06</v>
       </c>
-      <c r="E45" s="26">
+      <c r="E45" s="23">
         <v>1.0999999999999999E-2</v>
       </c>
-      <c r="F45" s="12" t="s">
+      <c r="F45" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="G45" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="H45" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="I45" s="10">
-        <v>2021</v>
-      </c>
-      <c r="J45" s="10">
+      <c r="G45" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="H45" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="I45" s="8">
+        <v>2021</v>
+      </c>
+      <c r="J45" s="8">
         <v>2022</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A46" s="15" t="s">
+      <c r="A46" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="B46" s="16" t="s">
+      <c r="B46" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="C46" s="21">
+      <c r="C46" s="20">
         <v>1357.3</v>
       </c>
-      <c r="D46" s="9">
+      <c r="D46" s="22">
         <v>0.106</v>
       </c>
-      <c r="E46" s="26">
+      <c r="E46" s="23">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="F46" s="12" t="s">
+      <c r="F46" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="G46" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="H46" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="I46" s="10">
-        <v>2021</v>
-      </c>
-      <c r="J46" s="10">
+      <c r="G46" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="H46" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="I46" s="8">
+        <v>2021</v>
+      </c>
+      <c r="J46" s="8">
         <v>2022</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A47" s="15" t="s">
+      <c r="A47" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="B47" s="16" t="s">
+      <c r="B47" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="C47" s="21">
+      <c r="C47" s="20">
         <v>1717</v>
       </c>
-      <c r="D47" s="9">
+      <c r="D47" s="22">
         <v>0.16</v>
       </c>
-      <c r="E47" s="26">
+      <c r="E47" s="23">
         <v>2.3E-2</v>
       </c>
-      <c r="F47" s="12" t="s">
+      <c r="F47" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="G47" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="H47" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="I47" s="10">
-        <v>2021</v>
-      </c>
-      <c r="J47" s="10">
+      <c r="G47" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="H47" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="I47" s="8">
+        <v>2021</v>
+      </c>
+      <c r="J47" s="8">
         <v>2022</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A48" s="15" t="s">
+      <c r="A48" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="B48" s="16" t="s">
+      <c r="B48" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="C48" s="21">
+      <c r="C48" s="20">
         <v>1798.8</v>
       </c>
-      <c r="D48" s="9">
+      <c r="D48" s="22">
         <v>0.17199999999999999</v>
       </c>
-      <c r="E48" s="26">
+      <c r="E48" s="23">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="F48" s="12" t="s">
+      <c r="F48" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="G48" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="H48" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="I48" s="10">
-        <v>2021</v>
-      </c>
-      <c r="J48" s="10">
+      <c r="G48" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="H48" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="I48" s="8">
+        <v>2021</v>
+      </c>
+      <c r="J48" s="8">
         <v>2022</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A49" s="15" t="s">
+      <c r="A49" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="B49" s="16" t="s">
+      <c r="B49" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="C49" s="21">
+      <c r="C49" s="20">
         <v>1614.2</v>
       </c>
-      <c r="D49" s="9">
+      <c r="D49" s="22">
         <v>0.128</v>
       </c>
-      <c r="E49" s="26">
+      <c r="E49" s="23">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="F49" s="12" t="s">
+      <c r="F49" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="G49" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="H49" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="I49" s="10">
-        <v>2021</v>
-      </c>
-      <c r="J49" s="10">
+      <c r="G49" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="H49" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="I49" s="8">
+        <v>2021</v>
+      </c>
+      <c r="J49" s="8">
         <v>2022</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A50" s="15" t="s">
+      <c r="A50" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="B50" s="16" t="s">
+      <c r="B50" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="C50" s="21">
+      <c r="C50" s="20">
         <v>1926.2</v>
       </c>
-      <c r="D50" s="9">
+      <c r="D50" s="22">
         <v>0.20399999999999999</v>
       </c>
-      <c r="E50" s="26">
+      <c r="E50" s="23">
         <v>2.9000000000000001E-2</v>
       </c>
-      <c r="F50" s="12" t="s">
+      <c r="F50" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="G50" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="H50" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="I50" s="10">
-        <v>2021</v>
-      </c>
-      <c r="J50" s="10">
+      <c r="G50" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="H50" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="I50" s="8">
+        <v>2021</v>
+      </c>
+      <c r="J50" s="8">
         <v>2022</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A51" s="15" t="s">
+      <c r="A51" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="B51" s="16" t="s">
+      <c r="B51" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="C51" s="21">
+      <c r="C51" s="20">
         <v>1584.6</v>
       </c>
-      <c r="D51" s="9">
+      <c r="D51" s="22">
         <v>0.11600000000000001</v>
       </c>
-      <c r="E51" s="26">
+      <c r="E51" s="23">
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="F51" s="12" t="s">
+      <c r="F51" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="G51" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="H51" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="I51" s="10">
-        <v>2021</v>
-      </c>
-      <c r="J51" s="10">
+      <c r="G51" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="H51" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="I51" s="8">
+        <v>2021</v>
+      </c>
+      <c r="J51" s="8">
         <v>2022</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A52" s="15" t="s">
+      <c r="A52" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="B52" s="16" t="s">
+      <c r="B52" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="C52" s="21">
+      <c r="C52" s="20">
         <v>1177</v>
       </c>
-      <c r="D52" s="9">
+      <c r="D52" s="22">
         <v>6.6000000000000003E-2</v>
       </c>
-      <c r="E52" s="26">
+      <c r="E52" s="23">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="F52" s="12" t="s">
+      <c r="F52" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="G52" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="H52" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="I52" s="10">
-        <v>2021</v>
-      </c>
-      <c r="J52" s="10">
+      <c r="G52" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="H52" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="I52" s="8">
+        <v>2021</v>
+      </c>
+      <c r="J52" s="8">
         <v>2022</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A53" s="15" t="s">
+      <c r="A53" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="B53" s="16" t="s">
+      <c r="B53" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="C53" s="21">
+      <c r="C53" s="20">
         <v>1763.2</v>
       </c>
-      <c r="D53" s="9">
+      <c r="D53" s="22">
         <v>0.17899999999999999</v>
       </c>
-      <c r="E53" s="26">
+      <c r="E53" s="23">
         <v>2.5999999999999999E-2</v>
       </c>
-      <c r="F53" s="12" t="s">
+      <c r="F53" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="G53" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="H53" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="I53" s="10">
-        <v>2021</v>
-      </c>
-      <c r="J53" s="10">
+      <c r="G53" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="H53" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="I53" s="8">
+        <v>2021</v>
+      </c>
+      <c r="J53" s="8">
         <v>2022</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A54" s="15" t="s">
+      <c r="A54" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="B54" s="16" t="s">
+      <c r="B54" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="C54" s="21">
+      <c r="C54" s="20">
         <v>1384.6</v>
       </c>
-      <c r="D54" s="9">
+      <c r="D54" s="22">
         <v>0.10100000000000001</v>
       </c>
-      <c r="E54" s="26">
+      <c r="E54" s="23">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="F54" s="12" t="s">
+      <c r="F54" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="G54" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="H54" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="I54" s="10">
-        <v>2021</v>
-      </c>
-      <c r="J54" s="10">
+      <c r="G54" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="H54" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="I54" s="8">
+        <v>2021</v>
+      </c>
+      <c r="J54" s="8">
         <v>2022</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A55" s="15" t="s">
+      <c r="A55" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="B55" s="16" t="s">
+      <c r="B55" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="C55" s="21">
+      <c r="C55" s="20">
         <v>1636.2</v>
       </c>
-      <c r="D55" s="9">
+      <c r="D55" s="22">
         <v>0.151</v>
       </c>
-      <c r="E55" s="26">
+      <c r="E55" s="23">
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="F55" s="12" t="s">
+      <c r="F55" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="G55" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="H55" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="I55" s="10">
-        <v>2021</v>
-      </c>
-      <c r="J55" s="10">
+      <c r="G55" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="H55" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="I55" s="8">
+        <v>2021</v>
+      </c>
+      <c r="J55" s="8">
         <v>2022</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A56" s="15" t="s">
+      <c r="A56" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="B56" s="16" t="s">
+      <c r="B56" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="C56" s="21">
+      <c r="C56" s="20">
         <v>1357</v>
       </c>
-      <c r="D56" s="9">
+      <c r="D56" s="22">
         <v>0.11600000000000001</v>
       </c>
-      <c r="E56" s="26">
+      <c r="E56" s="23">
         <v>1.6E-2</v>
       </c>
-      <c r="F56" s="12" t="s">
+      <c r="F56" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="G56" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="H56" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="I56" s="10">
-        <v>2021</v>
-      </c>
-      <c r="J56" s="10">
+      <c r="G56" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="H56" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="I56" s="8">
+        <v>2021</v>
+      </c>
+      <c r="J56" s="8">
         <v>2022</v>
       </c>
     </row>
     <row r="57" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="17" t="s">
+      <c r="A57" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="B57" s="18" t="s">
+      <c r="B57" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="C57" s="23">
+      <c r="C57" s="21">
         <v>1410</v>
       </c>
-      <c r="D57" s="24">
+      <c r="D57" s="26">
         <v>0.11</v>
       </c>
-      <c r="E57" s="28">
+      <c r="E57" s="27">
         <v>1.6E-2</v>
       </c>
-      <c r="F57" s="12" t="s">
+      <c r="F57" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="G57" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="H57" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="I57" s="10">
-        <v>2021</v>
-      </c>
-      <c r="J57" s="10">
+      <c r="G57" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="H57" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="I57" s="8">
+        <v>2021</v>
+      </c>
+      <c r="J57" s="8">
         <v>2022</v>
       </c>
     </row>

</xml_diff>